<commit_message>
commit code import/export excel
</commit_message>
<xml_diff>
--- a/SourceCode/HRManagement/HRManagement/Template/TemplateStaff.xlsx
+++ b/SourceCode/HRManagement/HRManagement/Template/TemplateStaff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SourceCode\HRManagement\SourceCode\HRManagement\HRManagement\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F44CFC1-67E1-4A1C-AF6A-F71537198988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3415CBE-03B9-4CFB-80AE-43E149007823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{427A5032-DE58-4655-91F0-8B92AB270E62}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{427A5032-DE58-4655-91F0-8B92AB270E62}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>STT</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Giới tính</t>
+  </si>
+  <si>
+    <t>Tài khoản*</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -666,34 +687,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE163415-3B84-4C13-9966-FB12B0F0D596}" name="Table1" displayName="Table1" ref="A1:Y40" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:Y40" xr:uid="{DE163415-3B84-4C13-9966-FB12B0F0D596}"/>
-  <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{E6B956C1-D173-4B05-B48C-A72F9F89CAC7}" name="STT" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{44A4560E-2199-4835-A186-C0ED0CB8BE2D}" name="Mã nhân viên*" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{DFE31C29-E3F3-4C3C-98D1-5661C0D6B335}" name="Tên nhân viên*" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{0A10DAC3-6DA8-4F4E-9EF3-B88B48BEA007}" name="Phòng ban*" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{E0E99004-E0FA-4D01-88EA-8F3F7C7C9FB4}" name="Vị trí*" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{22C80B7C-3901-4F81-ACA2-47EF6F01D7B8}" name="Ngày sinh" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{3FF7300A-05A4-4581-BB84-4925F82894A3}" name="Địa chỉ" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{06BAAC04-9BE1-4572-B7C1-5C50BE0F743E}" name="Dân tộc*" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{D149065C-6FD2-4AD9-B79E-9EFE059F9619}" name="Học vấn*" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{0D440826-6315-4D24-B999-607245F9395D}" name="Chuyên môn*" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{2BF5026D-A812-4700-A7CA-079EAA5AD6E9}" name="Email*" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{4FC36200-B2D0-4581-8128-0B76C3427664}" name="Số CCCD" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{C9A335E4-7CE2-4EC1-804A-270BC9444E29}" name="Ngày cấp" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{4A1A4E8A-76B3-4ABC-ABD5-04F30534AF5D}" name="Nơi cấp" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{6E8D2438-1115-41AF-B979-BC11BCC98062}" name="Giới tính" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{C6A38102-A358-417C-89A4-11AEF39055F4}" name="Số ĐT" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{754B48DF-852E-4F8A-B034-23D821B4A34A}" name="Loại HĐ" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{366D08EB-4BB4-482B-B7D5-865A9B5B0EE7}" name="Số HĐ" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{E59FEF4C-A335-4634-94D9-A9C013A6A46E}" name="Tên HĐ" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{4A8535DB-EB78-429F-8D02-B546B9F0F975}" name="Ngày BĐ" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{F7CC31C4-0F8E-43BE-8874-DC3B75F955B0}" name="Ngày HH" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{9CCCD986-535E-414B-87B1-EC80BB63D5AD}" name="Lương" dataDxfId="3"/>
-    <tableColumn id="23" xr3:uid="{287F2332-2E90-4F88-A797-8FDCEBF35C72}" name="Phụ cấp" dataDxfId="2"/>
-    <tableColumn id="24" xr3:uid="{5AFD47CD-AA75-462A-9BC7-C9D2CDE7B1F8}" name="Thuế TN" dataDxfId="1"/>
-    <tableColumn id="25" xr3:uid="{F257F840-D416-4B42-AD60-11744F55AA3B}" name="HS Lương" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DE163415-3B84-4C13-9966-FB12B0F0D596}" name="Table1" displayName="Table1" ref="A1:Z40" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:Z40" xr:uid="{DE163415-3B84-4C13-9966-FB12B0F0D596}"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{E6B956C1-D173-4B05-B48C-A72F9F89CAC7}" name="STT" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{44A4560E-2199-4835-A186-C0ED0CB8BE2D}" name="Mã nhân viên*" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{DFE31C29-E3F3-4C3C-98D1-5661C0D6B335}" name="Tên nhân viên*" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{0A10DAC3-6DA8-4F4E-9EF3-B88B48BEA007}" name="Phòng ban*" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{E0E99004-E0FA-4D01-88EA-8F3F7C7C9FB4}" name="Vị trí*" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{22C80B7C-3901-4F81-ACA2-47EF6F01D7B8}" name="Ngày sinh" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{3FF7300A-05A4-4581-BB84-4925F82894A3}" name="Địa chỉ" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{06BAAC04-9BE1-4572-B7C1-5C50BE0F743E}" name="Dân tộc*" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{D149065C-6FD2-4AD9-B79E-9EFE059F9619}" name="Học vấn*" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{0D440826-6315-4D24-B999-607245F9395D}" name="Chuyên môn*" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{2BF5026D-A812-4700-A7CA-079EAA5AD6E9}" name="Email*" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{4FC36200-B2D0-4581-8128-0B76C3427664}" name="Số CCCD" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{C9A335E4-7CE2-4EC1-804A-270BC9444E29}" name="Ngày cấp" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{4A1A4E8A-76B3-4ABC-ABD5-04F30534AF5D}" name="Nơi cấp" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{6E8D2438-1115-41AF-B979-BC11BCC98062}" name="Giới tính" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{C6A38102-A358-417C-89A4-11AEF39055F4}" name="Số ĐT" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{754B48DF-852E-4F8A-B034-23D821B4A34A}" name="Loại HĐ" dataDxfId="9"/>
+    <tableColumn id="18" xr3:uid="{366D08EB-4BB4-482B-B7D5-865A9B5B0EE7}" name="Số HĐ" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{E59FEF4C-A335-4634-94D9-A9C013A6A46E}" name="Tên HĐ" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{4A8535DB-EB78-429F-8D02-B546B9F0F975}" name="Ngày BĐ" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{F7CC31C4-0F8E-43BE-8874-DC3B75F955B0}" name="Ngày HH" dataDxfId="5"/>
+    <tableColumn id="22" xr3:uid="{9CCCD986-535E-414B-87B1-EC80BB63D5AD}" name="Lương" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{287F2332-2E90-4F88-A797-8FDCEBF35C72}" name="Phụ cấp" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{5AFD47CD-AA75-462A-9BC7-C9D2CDE7B1F8}" name="Thuế TN" dataDxfId="2"/>
+    <tableColumn id="25" xr3:uid="{F257F840-D416-4B42-AD60-11744F55AA3B}" name="HS Lương" dataDxfId="1"/>
+    <tableColumn id="26" xr3:uid="{F89018F4-BF2D-4675-9427-5317E0150A1A}" name="Tài khoản*" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -996,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1074641B-D419-47A7-8AB3-1E149DCF9765}">
-  <dimension ref="A1:Y40"/>
+  <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1028,10 +1050,11 @@
     <col min="22" max="23" width="12" style="1" customWidth="1"/>
     <col min="24" max="24" width="11.77734375" style="1" customWidth="1"/>
     <col min="25" max="25" width="8.88671875" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.88671875" style="1"/>
+    <col min="26" max="26" width="11.21875" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1107,8 +1130,11 @@
       <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
       <c r="M2" s="4"/>
@@ -1118,46 +1144,46 @@
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>